<commit_message>
finalized project for submission
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -7,9 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="straight road 2 lanes" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="junction road 1 lane" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Accidents" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="junction road 1 lane" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Accidents" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,70 +452,265 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Vehicles passing through plus-junction</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. time (seconds) waited to enter junction</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 3, Direction 1)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 1, Direction 1)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 2, Direction 0)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 3, Direction 0)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 2, Direction 1)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>Avg. Speed (Road 1, Direction 0)</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Speed (Road 1, Direction 1)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-09-12 00:19:20</t>
+          <t>2024-09-12 12:54:21</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>161.1162816825348</v>
+        <v>45.92926081650629</v>
       </c>
       <c r="C2" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D2" t="n">
-        <v>162.7848233070203</v>
-      </c>
-      <c r="E2" t="n">
-        <v>159.4477400580494</v>
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>41.95354760787764</v>
+      </c>
+      <c r="G2" t="n">
+        <v>38.34384431504669</v>
+      </c>
+      <c r="H2" t="n">
+        <v>50.48263156737443</v>
+      </c>
+      <c r="I2" t="n">
+        <v>53.65087570321979</v>
+      </c>
+      <c r="J2" t="n">
+        <v>46.90326942537587</v>
+      </c>
+      <c r="K2" t="n">
+        <v>30.99240203369217</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-09-12 00:19:25</t>
+          <t>2024-09-12 12:54:26</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>146.1543488154065</v>
+        <v>41.82138950610611</v>
       </c>
       <c r="C3" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D3" t="n">
-        <v>137.7376995427169</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>154.5709980880962</v>
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>47.02869459013218</v>
+      </c>
+      <c r="G3" t="n">
+        <v>42.10725220665784</v>
+      </c>
+      <c r="H3" t="n">
+        <v>48.22473030506848</v>
+      </c>
+      <c r="I3" t="n">
+        <v>31.9789586431459</v>
+      </c>
+      <c r="J3" t="n">
+        <v>45.34156649943344</v>
+      </c>
+      <c r="K3" t="n">
+        <v>39.26533037673937</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-09-12 00:19:28</t>
+          <t>2024-09-12 12:54:31</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>148.4359240267293</v>
+        <v>26.39248297375177</v>
       </c>
       <c r="C4" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" t="n">
-        <v>145.3238638626348</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>155.9048684205562</v>
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>49.74096206497433</v>
+      </c>
+      <c r="G4" t="n">
+        <v>21.42495997551785</v>
+      </c>
+      <c r="H4" t="n">
+        <v>32.75092417349077</v>
+      </c>
+      <c r="I4" t="n">
+        <v>32.52575578686218</v>
+      </c>
+      <c r="J4" t="n">
+        <v>38.0290474530395</v>
+      </c>
+      <c r="K4" t="n">
+        <v>7.42667733007719</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-09-12 12:54:36</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>25.03843167758055</v>
+      </c>
+      <c r="C5" t="n">
+        <v>21</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3.944177707036336</v>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="n">
+        <v>14.95648037370953</v>
+      </c>
+      <c r="H5" t="n">
+        <v>28.45176961923142</v>
+      </c>
+      <c r="I5" t="n">
+        <v>20.14438890706975</v>
+      </c>
+      <c r="J5" t="n">
+        <v>40.45928231039007</v>
+      </c>
+      <c r="K5" t="n">
+        <v>34.85205470129428</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-09-12 12:54:41</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>26.30578583125924</v>
+      </c>
+      <c r="C6" t="n">
+        <v>25</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2.372208913167318</v>
+      </c>
+      <c r="F6" t="n">
+        <v>43.74168849645782</v>
+      </c>
+      <c r="G6" t="n">
+        <v>14.89329178142397</v>
+      </c>
+      <c r="H6" t="n">
+        <v>40.76747288107121</v>
+      </c>
+      <c r="I6" t="n">
+        <v>23.854166384772</v>
+      </c>
+      <c r="J6" t="n">
+        <v>34.48049024965424</v>
+      </c>
+      <c r="K6" t="n">
+        <v>18.46908638619662</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-09-12 12:54:43</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>31.36618913223004</v>
+      </c>
+      <c r="C7" t="n">
+        <v>27</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5.60251796245575</v>
+      </c>
+      <c r="F7" t="n">
+        <v>40.05089939801602</v>
+      </c>
+      <c r="G7" t="n">
+        <v>29.07666659567725</v>
+      </c>
+      <c r="H7" t="n">
+        <v>45.39314725642101</v>
+      </c>
+      <c r="I7" t="n">
+        <v>19.03136042200451</v>
+      </c>
+      <c r="J7" t="n">
+        <v>38.77237372484483</v>
+      </c>
+      <c r="K7" t="n">
+        <v>27.42432049445251</v>
       </c>
     </row>
   </sheetData>
@@ -530,7 +724,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,351 +740,23 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Average Speed (km\h)</t>
+          <t>Road Type</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Density</t>
+          <t>Vehicle Types</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Vehicles passing through plus-junction</t>
+          <t>Speeds At Crash Time (km\h)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Avg. time (seconds) waited to enter junction</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Speed (Road 3, Direction 1)</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Speed (Road 1, Direction 1)</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Speed (Road 2, Direction 0)</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Speed (Road 2, Direction 1)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Speed (Road 3, Direction 0)</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Speed (Road 1, Direction 0)</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2024-09-12 00:19:37</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>42.8606609419605</v>
-      </c>
-      <c r="C2" t="n">
-        <v>10</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>43.04406275200475</v>
-      </c>
-      <c r="G2" t="n">
-        <v>45.29653875857061</v>
-      </c>
-      <c r="H2" t="n">
-        <v>47.20553516739295</v>
-      </c>
-      <c r="I2" t="n">
-        <v>39.09511680989982</v>
-      </c>
-      <c r="J2" t="n">
-        <v>44.68036264557358</v>
-      </c>
-      <c r="K2" t="n">
-        <v>33.00743990472633</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2024-09-12 00:19:42</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>44.2026346888154</v>
-      </c>
-      <c r="C3" t="n">
-        <v>15</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>43.40041155588791</v>
-      </c>
-      <c r="G3" t="n">
-        <v>53.27771125253204</v>
-      </c>
-      <c r="H3" t="n">
-        <v>43.54044219736036</v>
-      </c>
-      <c r="I3" t="n">
-        <v>39.69272417462864</v>
-      </c>
-      <c r="J3" t="n">
-        <v>48.67484055554703</v>
-      </c>
-      <c r="K3" t="n">
-        <v>30.18713342743979</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2024-09-12 00:19:47</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>40.36883543235182</v>
-      </c>
-      <c r="C4" t="n">
-        <v>16</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>35.83575265107249</v>
-      </c>
-      <c r="G4" t="n">
-        <v>74.04536030232616</v>
-      </c>
-      <c r="H4" t="n">
-        <v>43.1533373902775</v>
-      </c>
-      <c r="I4" t="n">
-        <v>39.93990832632662</v>
-      </c>
-      <c r="J4" t="n">
-        <v>41.81842762612849</v>
-      </c>
-      <c r="K4" t="n">
-        <v>20.23885813427707</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2024-09-12 00:19:48</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>45.0899462937592</v>
-      </c>
-      <c r="C5" t="n">
-        <v>18</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>35.83575265107249</v>
-      </c>
-      <c r="G5" t="n">
-        <v>100.0574294943651</v>
-      </c>
-      <c r="H5" t="n">
-        <v>42.69856402940746</v>
-      </c>
-      <c r="I5" t="n">
-        <v>39.93990832632662</v>
-      </c>
-      <c r="J5" t="n">
-        <v>47.56054001512872</v>
-      </c>
-      <c r="K5" t="n">
-        <v>19.65884261322199</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Time Stamp</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Road Type</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Vehicle Types</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Speeds At Crash Time (km\h)</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>Accident ID</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2024-09-12 00:19:27</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>straight</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Car and Car</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>77.74 and 166.83</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2024-09-12 00:19:28</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>straight</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Car and Truck</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>0.00 and 78.01</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2024-09-12 00:19:45</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>junction</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Car and Truck</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>18.99 and 47.32</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2024-09-12 00:19:46</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>junction</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Car and Truck</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>130.85 and 0.00</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed SimulationManager to SimulationInitiator
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -7,8 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="junction road 1 lane" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Accidents" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="straight road 2 lanes" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="roundabout road 1 lane" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="junction road 1 lane" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Accidents" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,265 +454,32 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Vehicles passing through plus-junction</t>
+          <t>Avg. Speed (Road 1, Direction 0)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Avg. time (seconds) waited to enter junction</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Speed (Road 3, Direction 1)</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
           <t>Avg. Speed (Road 1, Direction 1)</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Speed (Road 2, Direction 0)</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Speed (Road 3, Direction 0)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Speed (Road 2, Direction 1)</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Avg. Speed (Road 1, Direction 0)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-09-12 12:54:21</t>
+          <t>2024-09-12 13:39:59</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>45.92926081650629</v>
+        <v>73.61354638096506</v>
       </c>
       <c r="C2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>41.95354760787764</v>
-      </c>
-      <c r="G2" t="n">
-        <v>38.34384431504669</v>
-      </c>
-      <c r="H2" t="n">
-        <v>50.48263156737443</v>
-      </c>
-      <c r="I2" t="n">
-        <v>53.65087570321979</v>
-      </c>
-      <c r="J2" t="n">
-        <v>46.90326942537587</v>
-      </c>
-      <c r="K2" t="n">
-        <v>30.99240203369217</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2024-09-12 12:54:26</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>41.82138950610611</v>
-      </c>
-      <c r="C3" t="n">
-        <v>15</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>47.02869459013218</v>
-      </c>
-      <c r="G3" t="n">
-        <v>42.10725220665784</v>
-      </c>
-      <c r="H3" t="n">
-        <v>48.22473030506848</v>
-      </c>
-      <c r="I3" t="n">
-        <v>31.9789586431459</v>
-      </c>
-      <c r="J3" t="n">
-        <v>45.34156649943344</v>
-      </c>
-      <c r="K3" t="n">
-        <v>39.26533037673937</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2024-09-12 12:54:31</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>26.39248297375177</v>
-      </c>
-      <c r="C4" t="n">
-        <v>18</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>49.74096206497433</v>
-      </c>
-      <c r="G4" t="n">
-        <v>21.42495997551785</v>
-      </c>
-      <c r="H4" t="n">
-        <v>32.75092417349077</v>
-      </c>
-      <c r="I4" t="n">
-        <v>32.52575578686218</v>
-      </c>
-      <c r="J4" t="n">
-        <v>38.0290474530395</v>
-      </c>
-      <c r="K4" t="n">
-        <v>7.42667733007719</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2024-09-12 12:54:36</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>25.03843167758055</v>
-      </c>
-      <c r="C5" t="n">
-        <v>21</v>
-      </c>
-      <c r="D5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" t="n">
-        <v>3.944177707036336</v>
-      </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="n">
-        <v>14.95648037370953</v>
-      </c>
-      <c r="H5" t="n">
-        <v>28.45176961923142</v>
-      </c>
-      <c r="I5" t="n">
-        <v>20.14438890706975</v>
-      </c>
-      <c r="J5" t="n">
-        <v>40.45928231039007</v>
-      </c>
-      <c r="K5" t="n">
-        <v>34.85205470129428</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2024-09-12 12:54:41</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>26.30578583125924</v>
-      </c>
-      <c r="C6" t="n">
-        <v>25</v>
-      </c>
-      <c r="D6" t="n">
-        <v>3</v>
-      </c>
-      <c r="E6" t="n">
-        <v>2.372208913167318</v>
-      </c>
-      <c r="F6" t="n">
-        <v>43.74168849645782</v>
-      </c>
-      <c r="G6" t="n">
-        <v>14.89329178142397</v>
-      </c>
-      <c r="H6" t="n">
-        <v>40.76747288107121</v>
-      </c>
-      <c r="I6" t="n">
-        <v>23.854166384772</v>
-      </c>
-      <c r="J6" t="n">
-        <v>34.48049024965424</v>
-      </c>
-      <c r="K6" t="n">
-        <v>18.46908638619662</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2024-09-12 12:54:43</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>31.36618913223004</v>
-      </c>
-      <c r="C7" t="n">
-        <v>27</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>5.60251796245575</v>
-      </c>
-      <c r="F7" t="n">
-        <v>40.05089939801602</v>
-      </c>
-      <c r="G7" t="n">
-        <v>29.07666659567725</v>
-      </c>
-      <c r="H7" t="n">
-        <v>45.39314725642101</v>
-      </c>
-      <c r="I7" t="n">
-        <v>19.03136042200451</v>
-      </c>
-      <c r="J7" t="n">
-        <v>38.77237372484483</v>
-      </c>
-      <c r="K7" t="n">
-        <v>27.42432049445251</v>
+        <v>71.60265825820706</v>
+      </c>
+      <c r="E2" t="n">
+        <v>75.62443450372309</v>
       </c>
     </row>
   </sheetData>
@@ -719,6 +488,364 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Time Stamp</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Average Speed (km\h)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Density</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Vehicles passing through roundabout</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 1, Direction 0)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 1, Direction 1)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 2, Direction 0)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 2, Direction 1)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 3, Direction 0)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 3, Direction 1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2024-09-12 13:40:06</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>43.05990595936821</v>
+      </c>
+      <c r="C2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>38.19789495790369</v>
+      </c>
+      <c r="F2" t="n">
+        <v>45.15376236358112</v>
+      </c>
+      <c r="G2" t="n">
+        <v>38.09917333663068</v>
+      </c>
+      <c r="H2" t="n">
+        <v>43.56371066725747</v>
+      </c>
+      <c r="I2" t="n">
+        <v>47.80462216009933</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-09-12 13:40:11</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>41.09231221825002</v>
+      </c>
+      <c r="C3" t="n">
+        <v>14</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>34.37745744802951</v>
+      </c>
+      <c r="F3" t="n">
+        <v>41.19047329164647</v>
+      </c>
+      <c r="G3" t="n">
+        <v>38.40769515612099</v>
+      </c>
+      <c r="H3" t="n">
+        <v>42.82934853098349</v>
+      </c>
+      <c r="I3" t="n">
+        <v>45.44054132490948</v>
+      </c>
+      <c r="J3" t="n">
+        <v>49.79286748753488</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-09-12 13:40:16</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>37.44534878161553</v>
+      </c>
+      <c r="C4" t="n">
+        <v>18</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>39.34427745860437</v>
+      </c>
+      <c r="F4" t="n">
+        <v>35.55341877121457</v>
+      </c>
+      <c r="G4" t="n">
+        <v>40.32162784312454</v>
+      </c>
+      <c r="H4" t="n">
+        <v>38.47664114739003</v>
+      </c>
+      <c r="I4" t="n">
+        <v>30.96543789644304</v>
+      </c>
+      <c r="J4" t="n">
+        <v>49.79286748753488</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-09-12 13:40:17</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>36.69997140249792</v>
+      </c>
+      <c r="C5" t="n">
+        <v>21</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>38.49806409187927</v>
+      </c>
+      <c r="F5" t="n">
+        <v>37.60123964249841</v>
+      </c>
+      <c r="G5" t="n">
+        <v>27.70535214057742</v>
+      </c>
+      <c r="H5" t="n">
+        <v>33.72485095841363</v>
+      </c>
+      <c r="I5" t="n">
+        <v>43.11754128901119</v>
+      </c>
+      <c r="J5" t="n">
+        <v>45.43964350847895</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Time Stamp</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Average Speed (km\h)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Density</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Vehicles passing through plus-junction</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. time (seconds) waited to enter junction</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 3, Direction 1)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 1, Direction 1)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 2, Direction 0)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 2, Direction 1)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 3, Direction 0)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Avg. Speed (Road 1, Direction 0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2024-09-12 13:40:24</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>46.75327837037735</v>
+      </c>
+      <c r="C2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>59.65951516723347</v>
+      </c>
+      <c r="G2" t="n">
+        <v>47.13881959706224</v>
+      </c>
+      <c r="H2" t="n">
+        <v>36.35208980093715</v>
+      </c>
+      <c r="I2" t="n">
+        <v>47.04397004973643</v>
+      </c>
+      <c r="J2" t="n">
+        <v>50.27218517418505</v>
+      </c>
+      <c r="K2" t="n">
+        <v>35.85795072325808</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-09-12 13:40:26</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>46.97671717024681</v>
+      </c>
+      <c r="C3" t="n">
+        <v>11</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>59.65951516723347</v>
+      </c>
+      <c r="G3" t="n">
+        <v>47.13881959706224</v>
+      </c>
+      <c r="H3" t="n">
+        <v>43.41466619973752</v>
+      </c>
+      <c r="I3" t="n">
+        <v>47.04397004973643</v>
+      </c>
+      <c r="J3" t="n">
+        <v>50.27218517418505</v>
+      </c>
+      <c r="K3" t="n">
+        <v>40.67254583201941</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>